<commit_message>
Add mitigation & detection in execution stage
</commit_message>
<xml_diff>
--- a/Cyber Threat Dictionary/Cyber Threat Dictionary Draft.xlsx
+++ b/Cyber Threat Dictionary/Cyber Threat Dictionary Draft.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Enterprise ATT&amp;CK (v11)" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Notepad" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="150">
   <si>
     <t xml:space="preserve">Reconnaissance</t>
   </si>
@@ -86,6 +86,12 @@
     <t xml:space="preserve">Antivirus/Antimalware</t>
   </si>
   <si>
+    <t xml:space="preserve">Account Manipulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-factor Authentication</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gather Victim Host Information</t>
   </si>
   <si>
@@ -98,6 +104,9 @@
     <t xml:space="preserve">Behavior Prevention on Endpoint</t>
   </si>
   <si>
+    <t xml:space="preserve">Network Segmentation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gather Victim Identity Information</t>
   </si>
   <si>
@@ -110,6 +119,9 @@
     <t xml:space="preserve">Code Signing</t>
   </si>
   <si>
+    <t xml:space="preserve">Operating System Configuration</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gather Victim Network Information</t>
   </si>
   <si>
@@ -122,6 +134,9 @@
     <t xml:space="preserve">Disable or Remove Feature or Program</t>
   </si>
   <si>
+    <t xml:space="preserve">Privileged Account Management</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gather Victim Org Information</t>
   </si>
   <si>
@@ -137,6 +152,9 @@
     <t xml:space="preserve">Execution Prevention</t>
   </si>
   <si>
+    <t xml:space="preserve">Active Directory</t>
+  </si>
+  <si>
     <t xml:space="preserve">Phishing for Information</t>
   </si>
   <si>
@@ -146,7 +164,7 @@
     <t xml:space="preserve">File</t>
   </si>
   <si>
-    <t xml:space="preserve">Privileged Account Management</t>
+    <t xml:space="preserve">Command</t>
   </si>
   <si>
     <t xml:space="preserve">Search Closed Sources</t>
@@ -167,7 +185,7 @@
     <t xml:space="preserve">Process</t>
   </si>
   <si>
-    <t xml:space="preserve">Command</t>
+    <t xml:space="preserve">Group</t>
   </si>
   <si>
     <t xml:space="preserve">Search Open Websites/Domains</t>
@@ -182,39 +200,57 @@
     <t xml:space="preserve">Search Victim-Owned Websites</t>
   </si>
   <si>
-    <t xml:space="preserve">Network Segmentation</t>
+    <t xml:space="preserve">User Account</t>
   </si>
   <si>
     <t xml:space="preserve">Script</t>
   </si>
   <si>
+    <t xml:space="preserve">BITS Jobs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter Network Traffic</t>
+  </si>
+  <si>
     <t xml:space="preserve">Container Administration Command</t>
   </si>
   <si>
     <t xml:space="preserve">Limit Access to Resource Over Network</t>
   </si>
   <si>
+    <t xml:space="preserve">User Account Management</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vulnerability Scanning</t>
   </si>
   <si>
-    <t xml:space="preserve">User Account Management</t>
-  </si>
-  <si>
     <t xml:space="preserve">External Remote Services</t>
   </si>
   <si>
+    <t xml:space="preserve">Service</t>
+  </si>
+  <si>
     <t xml:space="preserve">Deploy Container</t>
   </si>
   <si>
     <t xml:space="preserve">Audit</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi-factor Authentication</t>
+    <t xml:space="preserve">Boot or Logon Autostart Execution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not easy to mitigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driver</t>
   </si>
   <si>
     <t xml:space="preserve">Logon Session</t>
   </si>
   <si>
+    <t xml:space="preserve">Kernel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Container</t>
   </si>
   <si>
@@ -230,12 +266,24 @@
     <t xml:space="preserve">Exploitation for Client Execution</t>
   </si>
   <si>
+    <t xml:space="preserve">Windows Registry</t>
+  </si>
+  <si>
     <t xml:space="preserve">Asset management systems</t>
   </si>
   <si>
+    <t xml:space="preserve">Boot or Logon Initialization Scripts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restrict File and Directory Permissions</t>
+  </si>
+  <si>
     <t xml:space="preserve">Endpoint sensors</t>
   </si>
   <si>
+    <t xml:space="preserve">Restrict Registry Permissions</t>
+  </si>
+  <si>
     <t xml:space="preserve">Phishing</t>
   </si>
   <si>
@@ -254,6 +302,12 @@
     <t xml:space="preserve">User Training</t>
   </si>
   <si>
+    <t xml:space="preserve">Browser Extensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limit Software Installation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Replication Through Removable Media</t>
   </si>
   <si>
@@ -269,12 +323,15 @@
     <t xml:space="preserve">Scheduled Task/Job</t>
   </si>
   <si>
-    <t xml:space="preserve">Operating System Configuration</t>
+    <t xml:space="preserve">Compromise Client Software Binary</t>
   </si>
   <si>
     <t xml:space="preserve">Checksum</t>
   </si>
   <si>
+    <t xml:space="preserve">Create Account</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trusted Relationship</t>
   </si>
   <si>
@@ -293,154 +350,127 @@
     <t xml:space="preserve">Shared Modules</t>
   </si>
   <si>
+    <t xml:space="preserve">Create or Modify System Process</t>
+  </si>
+  <si>
     <t xml:space="preserve">Software Deployment Tools</t>
   </si>
   <si>
     <t xml:space="preserve">Active Directory Configuration</t>
   </si>
   <si>
-    <t xml:space="preserve">User Account</t>
-  </si>
-  <si>
     <t xml:space="preserve">Remote Data Storage</t>
   </si>
   <si>
     <t xml:space="preserve">System Services</t>
   </si>
   <si>
-    <t xml:space="preserve">Restrict File and Directory Permissions</t>
+    <t xml:space="preserve">Event Triggered Execution</t>
   </si>
   <si>
     <t xml:space="preserve">Command Execution</t>
   </si>
   <si>
-    <t xml:space="preserve">Service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Windows Registry</t>
+    <t xml:space="preserve">WMI</t>
   </si>
   <si>
     <t xml:space="preserve">User Execution</t>
   </si>
   <si>
+    <t xml:space="preserve">Hijack Execution Flow</t>
+  </si>
+  <si>
     <t xml:space="preserve">Instance</t>
   </si>
   <si>
+    <t xml:space="preserve">Restrict Library Loading</t>
+  </si>
+  <si>
     <t xml:space="preserve">Windows Management Instrumentation</t>
   </si>
   <si>
-    <t xml:space="preserve">Application Log </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application Log Content </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitor for third-party application logging, messaging, and/or other artifacts that may rely upon specific actions by a user in order to gain execution.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS0017 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Command </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Command Execution </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitor the execution of and command-line arguments for applications that may be used by an adversary to gain Initial Access that require user interaction. This includes compression applications, such as those for zip files, that can be used to Deobfuscate/Decode Files or Information in payloads.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS0032 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Container </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Container Creation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitor for newly constructed containers that may use an existing, legitimate external Web service to exfiltrate data rather than their primary command and control channel.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Container Start </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitor for the activation or invocation of a container (ex: docker start or docker restart)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS0022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">File </t>
-  </si>
-  <si>
-    <t xml:space="preserve">File Creation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti-virus can potentially detect malicious documents and files that are downloaded and executed on the user's computer. Endpoint sensing or network sensing can potentially detect malicious events once the file is opened (such as a Microsoft Word document or PDF reaching out to the internet or spawning powershell.exe).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS0007 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image Creation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitor for newly constructed image that may use an existing, legitimate external Web service to exfiltrate data rather than their primary command and control channel.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS0030 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instance </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instance Creation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitor for newly constructed instances that may use an existing, legitimate external Web service to exfiltrate data rather than their primary command and control channel.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instance Start </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitor for the activation or invocation of an instance (ex: instance.start within GCP Audit Logs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS0029 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Network Traffic </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Network Connection Creation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitor for newly constructed web-based network connections that are sent to malicious or suspicious destinations (e.g. destinations attributed to phishing campaigns). Consider correlation with process monitoring and command line to detect anomalous processes execution and command line arguments (e.g. monitor anomalies in use of files that do not normally initiate network connections or unusual connections initiated by regsvr32.exe, rundll.exe, .SCF, HTA, MSI, DLLs, or msiexec.exe).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Network Traffic Content </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitor and analyze traffic patterns and packet inspection associated with web-based network connections that are sent to malicious or suspicious detinations (e.g. destinations attributed to phishing campaigns). Consider correlation with process monitoring and command line to detect anomalous processes execution and command line arguments (e.g. monitor anomalies in use of files that do not normally initiate network connections or unusual connections initiated by regsvr32.exe, rundll.exe, .SCF, HTA, MSI, DLLs, or msiexec.exe).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS0009 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Process </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Process Creation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitor for newly executed processes that may be used by an adversary to gain Initial Access that require user interaction. This includes compression applications, such as those for zip files, that can be used to Deobfuscate/Decode Files or Information in payloads.</t>
+    <t xml:space="preserve">Implant Internal Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify Authentication Process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Privileged Process Integrity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office Application Startup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-OS Boot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boot Integrity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firmware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server Software Component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic Signaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1047  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audit  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regularly check component software on critical services that adversaries may target for persistence to verify the integrity of the systems and identify if unexpected changes have been made.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1045  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code Signing  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensure all application component binaries are signed by the correct application developers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1042  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disable or Remove Feature or Program  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consider disabling software components from servers when possible to prevent abuse by adversaries.[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1026  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Privileged Account Management  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not allow administrator accounts that have permissions to add component software on these services to be used for day-to-day operations that may expose them to potential adversaries on unprivileged systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1024  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restrict Registry Permissions  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consider using Group Policy to configure and block modifications to service and other critical server parameters in the Registry.[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1018  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Account Management  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enforce the principle of least privilege by limiting privileges of user accounts so only authorized accounts can modify and/or add server software components.[3]</t>
   </si>
 </sst>
 </file>
@@ -584,10 +614,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R93"/>
+  <dimension ref="A1:T158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E75" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F87" activeCellId="0" sqref="F87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H135" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I152" activeCellId="0" sqref="I152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -613,34 +643,36 @@
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -669,9 +701,15 @@
       <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="I2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -681,24 +719,26 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -708,24 +748,26 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -735,24 +777,26 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -762,26 +806,30 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -791,24 +839,26 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -818,24 +868,26 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -845,24 +897,26 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -872,10 +926,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>17</v>
@@ -886,11 +940,13 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -900,22 +956,24 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -929,16 +987,22 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -951,20 +1015,22 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -977,16 +1043,18 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
@@ -996,16 +1064,20 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="3" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
@@ -1014,19 +1086,21 @@
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="N16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1035,154 +1109,188 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="N17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="4" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="3" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="3" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J22" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="0" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="3" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J23" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="0" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J24" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="0" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="4" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J25" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="0" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="0" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>17</v>
@@ -1190,41 +1298,57 @@
       <c r="H26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="3"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="0" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J27" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="0" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J28" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="0" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>17</v>
@@ -1235,229 +1359,328 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="0" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>74</v>
+        <v>90</v>
+      </c>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="0" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="0" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="0" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="3" t="s">
-        <v>75</v>
+        <v>91</v>
+      </c>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="4" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
+      </c>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="0" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="4" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F43" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="0" t="s">
-        <v>82</v>
+        <v>32</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="4"/>
       <c r="D45" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="I45" s="5"/>
+      <c r="J45" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1469,457 +1692,1237 @@
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K46" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="4" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="0" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="4"/>
       <c r="D49" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="0" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K50" s="0" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="4" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="0" t="s">
-        <v>87</v>
+        <v>106</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="0" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>17</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="0" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>91</v>
+        <v>111</v>
+      </c>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="4"/>
       <c r="D56" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="0" t="s">
-        <v>62</v>
+        <v>22</v>
+      </c>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="0" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="0" t="s">
-        <v>53</v>
+        <v>27</v>
+      </c>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="0" t="s">
-        <v>88</v>
+        <v>107</v>
+      </c>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="0" t="s">
-        <v>93</v>
+        <v>112</v>
+      </c>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K60" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="H62" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="0" t="s">
-        <v>76</v>
+        <v>92</v>
+      </c>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F64" s="5"/>
       <c r="G64" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
       <c r="H65" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F66" s="5" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K66" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K67" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="H68" s="0" t="s">
-        <v>95</v>
+        <v>84</v>
+      </c>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="H69" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F70" s="5"/>
       <c r="G70" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>96</v>
+        <v>115</v>
+      </c>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
       <c r="H71" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
       <c r="H72" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="0" t="s">
-        <v>97</v>
+        <v>68</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K73" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
       <c r="H74" s="0" t="s">
-        <v>98</v>
+        <v>81</v>
+      </c>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F75" s="5" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
       <c r="H77" s="0" t="s">
-        <v>72</v>
+        <v>88</v>
+      </c>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K77" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
       <c r="H78" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
       <c r="H79" s="0" t="s">
-        <v>76</v>
+        <v>92</v>
+      </c>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F80" s="5"/>
       <c r="G80" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K80" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
       <c r="H81" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
       <c r="H82" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="I83" s="5"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="0" t="s">
-        <v>100</v>
+        <v>119</v>
+      </c>
+      <c r="I84" s="5"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
       <c r="H85" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F87" s="5" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="I87" s="5"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F88" s="5"/>
       <c r="G88" s="5"/>
       <c r="H88" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
       <c r="H89" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="I89" s="5"/>
+      <c r="J89" s="5"/>
+      <c r="K89" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K90" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F91" s="5"/>
       <c r="G91" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="I91" s="5"/>
+      <c r="J91" s="5"/>
+      <c r="K91" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
       <c r="H93" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I94" s="5"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I95" s="5"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I96" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="J96" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K96" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I97" s="5"/>
+      <c r="J97" s="5"/>
+      <c r="K97" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I98" s="5"/>
+      <c r="J98" s="5"/>
+      <c r="K98" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I99" s="5"/>
+      <c r="J99" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K99" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I100" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J100" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K100" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I101" s="5"/>
+      <c r="J101" s="5"/>
+      <c r="K101" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I102" s="5"/>
+      <c r="J102" s="5"/>
+      <c r="K102" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I103" s="5"/>
+      <c r="J103" s="5"/>
+      <c r="K103" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I104" s="5"/>
+      <c r="J104" s="5"/>
+      <c r="K104" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I105" s="5"/>
+      <c r="J105" s="5"/>
+      <c r="K105" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I106" s="5"/>
+      <c r="J106" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K106" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I107" s="5"/>
+      <c r="J107" s="5"/>
+      <c r="K107" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I108" s="5"/>
+      <c r="J108" s="5"/>
+      <c r="K108" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I109" s="5"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I110" s="5"/>
+      <c r="J110" s="5"/>
+      <c r="K110" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I111" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J111" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K111" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I112" s="5"/>
+      <c r="J112" s="5"/>
+      <c r="K112" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I113" s="5"/>
+      <c r="J113" s="5"/>
+      <c r="K113" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I114" s="5"/>
+      <c r="J114" s="5"/>
+      <c r="K114" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I115" s="5"/>
+      <c r="J115" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K115" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I116" s="5"/>
+      <c r="J116" s="5"/>
+      <c r="K116" s="0" t="s">
         <v>47</v>
       </c>
     </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I117" s="5"/>
+      <c r="J117" s="5"/>
+      <c r="K117" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I118" s="5"/>
+      <c r="J118" s="5"/>
+      <c r="K118" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I119" s="5"/>
+      <c r="J119" s="5"/>
+      <c r="K119" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I120" s="5"/>
+      <c r="J120" s="5"/>
+      <c r="K120" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I121" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J121" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K121" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I122" s="5"/>
+      <c r="J122" s="5"/>
+      <c r="K122" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I123" s="5"/>
+      <c r="J123" s="5"/>
+      <c r="K123" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I124" s="5"/>
+      <c r="J124" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K124" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I125" s="5"/>
+      <c r="J125" s="5"/>
+      <c r="K125" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I126" s="5"/>
+      <c r="J126" s="5"/>
+      <c r="K126" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I127" s="5"/>
+      <c r="J127" s="5"/>
+      <c r="K127" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I128" s="5"/>
+      <c r="J128" s="5"/>
+      <c r="K128" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I129" s="5"/>
+      <c r="J129" s="5"/>
+      <c r="K129" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I130" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J130" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K130" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I131" s="5"/>
+      <c r="J131" s="5"/>
+      <c r="K131" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I132" s="5"/>
+      <c r="J132" s="5"/>
+      <c r="K132" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I133" s="5"/>
+      <c r="J133" s="5"/>
+      <c r="K133" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I134" s="5"/>
+      <c r="J134" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K134" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I135" s="5"/>
+      <c r="J135" s="5"/>
+      <c r="K135" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I136" s="5"/>
+      <c r="J136" s="5"/>
+      <c r="K136" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I137" s="5"/>
+      <c r="J137" s="5"/>
+      <c r="K137" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I138" s="5"/>
+      <c r="J138" s="5"/>
+      <c r="K138" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I139" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J139" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K139" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I140" s="5"/>
+      <c r="J140" s="5"/>
+      <c r="K140" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I141" s="5"/>
+      <c r="J141" s="5"/>
+      <c r="K141" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I142" s="5"/>
+      <c r="J142" s="5"/>
+      <c r="K142" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I143" s="5"/>
+      <c r="J143" s="5"/>
+      <c r="K143" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I144" s="5"/>
+      <c r="J144" s="5"/>
+      <c r="K144" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I145" s="5"/>
+      <c r="J145" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K145" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I146" s="5"/>
+      <c r="J146" s="5"/>
+      <c r="K146" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I147" s="5"/>
+      <c r="J147" s="5"/>
+      <c r="K147" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I148" s="5"/>
+      <c r="J148" s="5"/>
+      <c r="K148" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I149" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="J149" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K149" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I150" s="5"/>
+      <c r="J150" s="5"/>
+      <c r="K150" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I151" s="5"/>
+      <c r="J151" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K151" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I152" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J152" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K152" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I153" s="5"/>
+      <c r="J153" s="5"/>
+      <c r="K153" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I154" s="5"/>
+      <c r="J154" s="5"/>
+      <c r="K154" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I155" s="5"/>
+      <c r="J155" s="5"/>
+      <c r="K155" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I156" s="5"/>
+      <c r="J156" s="5"/>
+      <c r="K156" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I157" s="5"/>
+      <c r="J157" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K157" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K158" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="115">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="F2:F12"/>
     <mergeCell ref="G2:G8"/>
+    <mergeCell ref="I2:I11"/>
+    <mergeCell ref="J2:J5"/>
     <mergeCell ref="D6:D9"/>
+    <mergeCell ref="J6:J11"/>
     <mergeCell ref="G9:G12"/>
     <mergeCell ref="C10:C17"/>
     <mergeCell ref="D10:D15"/>
+    <mergeCell ref="I12:I18"/>
+    <mergeCell ref="J12:J14"/>
     <mergeCell ref="F13:F18"/>
     <mergeCell ref="G13:G16"/>
+    <mergeCell ref="J15:J18"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="G17:G18"/>
     <mergeCell ref="C18:C24"/>
     <mergeCell ref="D18:D21"/>
     <mergeCell ref="F19:F25"/>
     <mergeCell ref="G19:G22"/>
+    <mergeCell ref="I19:I26"/>
+    <mergeCell ref="J20:J26"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="G23:G25"/>
     <mergeCell ref="C25:C28"/>
@@ -1927,45 +2930,87 @@
     <mergeCell ref="F26:F29"/>
     <mergeCell ref="G26:G27"/>
     <mergeCell ref="D27:D28"/>
+    <mergeCell ref="I27:I33"/>
+    <mergeCell ref="J27:J28"/>
     <mergeCell ref="G28:G29"/>
     <mergeCell ref="C29:C36"/>
     <mergeCell ref="D29:D33"/>
+    <mergeCell ref="J29:J33"/>
     <mergeCell ref="F30:F38"/>
     <mergeCell ref="G30:G35"/>
     <mergeCell ref="D34:D36"/>
+    <mergeCell ref="I34:I43"/>
+    <mergeCell ref="J34:J38"/>
     <mergeCell ref="G36:G38"/>
     <mergeCell ref="C37:C42"/>
     <mergeCell ref="D37:D39"/>
     <mergeCell ref="F39:F42"/>
     <mergeCell ref="G39:G40"/>
+    <mergeCell ref="J39:J43"/>
     <mergeCell ref="D40:D42"/>
     <mergeCell ref="G41:G42"/>
     <mergeCell ref="C43:C46"/>
     <mergeCell ref="D43:D44"/>
     <mergeCell ref="F43:F51"/>
     <mergeCell ref="G43:G46"/>
+    <mergeCell ref="I44:I45"/>
     <mergeCell ref="D45:D46"/>
+    <mergeCell ref="I46:I52"/>
+    <mergeCell ref="J46:J49"/>
     <mergeCell ref="C47:C50"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="G47:G51"/>
     <mergeCell ref="D49:D50"/>
+    <mergeCell ref="J50:J52"/>
     <mergeCell ref="C51:C57"/>
     <mergeCell ref="D51:D55"/>
     <mergeCell ref="F52:F54"/>
     <mergeCell ref="G53:G54"/>
+    <mergeCell ref="I53:I65"/>
+    <mergeCell ref="J53:J59"/>
     <mergeCell ref="F55:F65"/>
     <mergeCell ref="G55:G63"/>
     <mergeCell ref="D56:D57"/>
+    <mergeCell ref="J60:J65"/>
     <mergeCell ref="G64:G65"/>
     <mergeCell ref="F66:F74"/>
     <mergeCell ref="G66:G69"/>
+    <mergeCell ref="I66:I72"/>
+    <mergeCell ref="J67:J72"/>
     <mergeCell ref="G70:G74"/>
+    <mergeCell ref="I73:I79"/>
+    <mergeCell ref="J73:J76"/>
     <mergeCell ref="F75:F86"/>
     <mergeCell ref="G75:G79"/>
+    <mergeCell ref="J77:J79"/>
     <mergeCell ref="G80:G86"/>
+    <mergeCell ref="I80:I95"/>
+    <mergeCell ref="J80:J89"/>
     <mergeCell ref="F87:F93"/>
     <mergeCell ref="G87:G90"/>
+    <mergeCell ref="J90:J95"/>
     <mergeCell ref="G91:G93"/>
+    <mergeCell ref="I96:I99"/>
+    <mergeCell ref="J96:J98"/>
+    <mergeCell ref="I100:I110"/>
+    <mergeCell ref="J100:J105"/>
+    <mergeCell ref="J106:J110"/>
+    <mergeCell ref="I111:I120"/>
+    <mergeCell ref="J111:J114"/>
+    <mergeCell ref="J115:J120"/>
+    <mergeCell ref="I121:I129"/>
+    <mergeCell ref="J121:J123"/>
+    <mergeCell ref="J124:J129"/>
+    <mergeCell ref="I130:I138"/>
+    <mergeCell ref="J130:J133"/>
+    <mergeCell ref="J134:J138"/>
+    <mergeCell ref="I139:I148"/>
+    <mergeCell ref="J139:J144"/>
+    <mergeCell ref="J145:J148"/>
+    <mergeCell ref="I149:I151"/>
+    <mergeCell ref="J149:J150"/>
+    <mergeCell ref="I152:I157"/>
+    <mergeCell ref="J152:J156"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1982,262 +3027,317 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+    <row r="1" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>137</v>
+      </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+    <row r="3" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+    <row r="4" customFormat="false" ht="344.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+    <row r="5" customFormat="false" ht="240.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+    <row r="6" customFormat="false" ht="255.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-    </row>
-    <row r="13" customFormat="false" ht="255.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="479.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="300" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="165.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="553.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="285.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="285.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="867.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="941.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="404.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>139</v>
-      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" display="Application Log"/>
-    <hyperlink ref="B13" r:id="rId2" location="Application%20Log%20Content" display="Application Log Content"/>
-    <hyperlink ref="A14" r:id="rId3" display="DS0017"/>
-    <hyperlink ref="B14" r:id="rId4" display="Command"/>
-    <hyperlink ref="C14" r:id="rId5" location="Command%20Execution" display="Command Execution"/>
-    <hyperlink ref="D14" r:id="rId6" display="Deobfuscate/Decode Files or Information"/>
-    <hyperlink ref="A15" r:id="rId7" display="DS0032"/>
-    <hyperlink ref="B15" r:id="rId8" display="Container"/>
-    <hyperlink ref="C15" r:id="rId9" location="Container%20Creation" display="Container Creation"/>
-    <hyperlink ref="C16" r:id="rId10" location="Container%20Start" display="Container Start"/>
-    <hyperlink ref="A17" r:id="rId11" display="DS0022"/>
-    <hyperlink ref="B17" r:id="rId12" display="File"/>
-    <hyperlink ref="C17" r:id="rId13" location="File%20Creation" display="File Creation"/>
-    <hyperlink ref="A18" r:id="rId14" display="DS0007"/>
-    <hyperlink ref="B18" r:id="rId15" display="Image"/>
-    <hyperlink ref="C18" r:id="rId16" location="Image%20Creation" display="Image Creation"/>
-    <hyperlink ref="A19" r:id="rId17" display="DS0030"/>
-    <hyperlink ref="B19" r:id="rId18" display="Instance"/>
-    <hyperlink ref="C19" r:id="rId19" location="Instance%20Creation" display="Instance Creation"/>
-    <hyperlink ref="C20" r:id="rId20" location="Instance%20Start" display="Instance Start"/>
-    <hyperlink ref="A21" r:id="rId21" display="DS0029"/>
-    <hyperlink ref="B21" r:id="rId22" display="Network Traffic"/>
-    <hyperlink ref="C21" r:id="rId23" location="Network%20Connection%20Creation" display="Network Connection Creation"/>
-    <hyperlink ref="C22" r:id="rId24" location="Network%20Traffic%20Content" display="Network Traffic Content"/>
-    <hyperlink ref="A23" r:id="rId25" display="DS0009"/>
-    <hyperlink ref="B23" r:id="rId26" display="Process"/>
-    <hyperlink ref="C23" r:id="rId27" location="Process%20Creation" display="Process Creation"/>
-    <hyperlink ref="D23" r:id="rId28" display="Deobfuscate/Decode Files or Information"/>
+    <hyperlink ref="A1" r:id="rId1" display="M1047 "/>
+    <hyperlink ref="B1" r:id="rId2" display="Audit "/>
+    <hyperlink ref="A2" r:id="rId3" display="M1045 "/>
+    <hyperlink ref="B2" r:id="rId4" display="Code Signing "/>
+    <hyperlink ref="A3" r:id="rId5" display="M1042 "/>
+    <hyperlink ref="B3" r:id="rId6" display="Disable or Remove Feature or Program "/>
+    <hyperlink ref="C3" r:id="rId7" display="[1]"/>
+    <hyperlink ref="A4" r:id="rId8" display="M1026 "/>
+    <hyperlink ref="B4" r:id="rId9" display="Privileged Account Management "/>
+    <hyperlink ref="A5" r:id="rId10" display="M1024 "/>
+    <hyperlink ref="B5" r:id="rId11" display="Restrict Registry Permissions "/>
+    <hyperlink ref="C5" r:id="rId12" display="[2]"/>
+    <hyperlink ref="A6" r:id="rId13" display="M1018 "/>
+    <hyperlink ref="B6" r:id="rId14" display="User Account Management "/>
+    <hyperlink ref="C6" r:id="rId15" display="[3]"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add mitigation & detection on Collection stage
</commit_message>
<xml_diff>
--- a/Cyber Threat Dictionary/Cyber Threat Dictionary Draft.xlsx
+++ b/Cyber Threat Dictionary/Cyber Threat Dictionary Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\507UAR\Desktop\Y4FinalReport\Cyber Threat Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147C8FBF-7000-40B7-B257-A43B9F273311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFF4FB4-E55F-42C1-9484-B76248A425B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23490" yWindow="1245" windowWidth="15375" windowHeight="7995" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="264">
   <si>
     <t>Reconnaissance</t>
   </si>
@@ -773,13 +773,58 @@
   </si>
   <si>
     <t>Monitor for an attempt by a user to gain access to a network or computing resource by providing web credentials (ex: Windows EID 1202) that may use alternate authentication material, such as password hashes, Kerberos tickets, and application access tokens, in order to move laterally within an environment and bypass normal system access controls.</t>
+  </si>
+  <si>
+    <t>Archive Collected Data</t>
+  </si>
+  <si>
+    <t>Audio Capture</t>
+  </si>
+  <si>
+    <t>Automated Collection</t>
+  </si>
+  <si>
+    <t>Browser Session Hijacking</t>
+  </si>
+  <si>
+    <t>Clipboard Data</t>
+  </si>
+  <si>
+    <t>Data from Cloud Storage Object</t>
+  </si>
+  <si>
+    <t>Data from Configuration Repository</t>
+  </si>
+  <si>
+    <t>Data from Information Repositories</t>
+  </si>
+  <si>
+    <t>Data from Local System</t>
+  </si>
+  <si>
+    <t>Data from Network Shared Drive</t>
+  </si>
+  <si>
+    <t>Data from Removable Media</t>
+  </si>
+  <si>
+    <t>Data Staged</t>
+  </si>
+  <si>
+    <t>Email Collection</t>
+  </si>
+  <si>
+    <t>Screen Capture</t>
+  </si>
+  <si>
+    <t>Video Capture</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -812,6 +857,12 @@
       <color rgb="FF212529"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -893,7 +944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -964,6 +1015,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1280,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD253"/>
+  <dimension ref="A1:AF253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,14 +1365,18 @@
     <col min="21" max="21" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="36" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="33" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="7" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" s="7" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1365,20 +1423,22 @@
       </c>
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
@@ -1457,8 +1517,18 @@
       <c r="Z2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD2" s="12"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
@@ -1507,8 +1577,16 @@
       <c r="Z3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD3" s="12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>38</v>
       </c>
@@ -1555,8 +1633,16 @@
       <c r="Z4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD4" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>44</v>
       </c>
@@ -1603,8 +1689,16 @@
       <c r="Z5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD5" s="12" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>50</v>
       </c>
@@ -1659,8 +1753,16 @@
       <c r="Z6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD6" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>58</v>
       </c>
@@ -1709,8 +1811,16 @@
       <c r="Z7" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD7" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>62</v>
       </c>
@@ -1761,8 +1871,16 @@
       <c r="Z8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD8" s="12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>67</v>
       </c>
@@ -1815,8 +1933,18 @@
       <c r="Z9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD9" s="12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>70</v>
       </c>
@@ -1868,8 +1996,16 @@
       <c r="Z10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD10" s="12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>73</v>
       </c>
@@ -1914,8 +2050,16 @@
       <c r="Z11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD11" s="12" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="4"/>
@@ -1974,8 +2118,16 @@
       <c r="Z12" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD12" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="4"/>
@@ -2032,8 +2184,11 @@
       <c r="Z13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AD13" s="12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="4"/>
@@ -2082,8 +2237,11 @@
       <c r="Z14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AD14" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="4"/>
@@ -2132,8 +2290,11 @@
       <c r="Z15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AD15" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="4"/>
@@ -2178,8 +2339,11 @@
       <c r="Z16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AD16" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="4"/>
@@ -2228,8 +2392,11 @@
       <c r="Z17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AD17" s="12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
         <v>91</v>
       </c>
@@ -2286,8 +2453,11 @@
       <c r="Z18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AD18" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="8" t="s">
@@ -2341,7 +2511,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="8" t="s">
@@ -2389,7 +2559,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="8" t="s">
@@ -2439,7 +2609,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
         <v>36</v>
@@ -2485,7 +2655,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="8" t="s">
@@ -2537,7 +2707,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="8" t="s">
@@ -2585,7 +2755,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
         <v>104</v>
       </c>
@@ -2639,7 +2809,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" t="s">
@@ -2689,7 +2859,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
         <v>36</v>
@@ -2739,7 +2909,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" t="s">
@@ -2789,7 +2959,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C29" s="4" t="s">
         <v>115</v>
       </c>
@@ -2843,7 +3013,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" t="s">
@@ -2893,7 +3063,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" t="s">
@@ -2947,7 +3117,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" t="s">
@@ -7662,9 +7832,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="392">
+  <mergeCells count="396">
     <mergeCell ref="Y64:Y68"/>
     <mergeCell ref="X62:X68"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="AA2:AA12"/>
+    <mergeCell ref="AB2:AB8"/>
+    <mergeCell ref="AB9:AB12"/>
     <mergeCell ref="Y42:Y44"/>
     <mergeCell ref="X39:X44"/>
     <mergeCell ref="Y45:Y53"/>

</xml_diff>

<commit_message>
Add mitigation & detection in exfiltration stage
</commit_message>
<xml_diff>
--- a/Cyber Threat Dictionary/Cyber Threat Dictionary Draft.xlsx
+++ b/Cyber Threat Dictionary/Cyber Threat Dictionary Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\507UAR\Desktop\Y4FinalReport\Cyber Threat Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C336F8-8307-4713-9657-1BB013E33C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F20F2F-0BAD-4A4C-AB68-74922CA46EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="290">
   <si>
     <t>Reconnaissance</t>
   </si>
@@ -866,6 +866,36 @@
   </si>
   <si>
     <t>SSL/TLS Inspection</t>
+  </si>
+  <si>
+    <t>Automated Exfiltration</t>
+  </si>
+  <si>
+    <t>Data Transfer Size Limits</t>
+  </si>
+  <si>
+    <t>Exfiltration Over Alternative Protocol</t>
+  </si>
+  <si>
+    <t>Exfiltration Over C2 Channel</t>
+  </si>
+  <si>
+    <t>Exfiltration Over Other Network Medium</t>
+  </si>
+  <si>
+    <t>Exfiltration Over Physical Medium</t>
+  </si>
+  <si>
+    <t>Exfiltration Over Web Service</t>
+  </si>
+  <si>
+    <t>Scheduled Transfer</t>
+  </si>
+  <si>
+    <t>Transfer Data to Cloud Account</t>
+  </si>
+  <si>
+    <t>FIle</t>
   </si>
 </sst>
 </file>
@@ -1409,10 +1439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH253"/>
+  <dimension ref="A1:AJ253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ49" sqref="AJ49"/>
+    <sheetView tabSelected="1" topLeftCell="AD25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ40" sqref="AJ40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,15 +1473,19 @@
     <col min="24" max="24" width="36" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="33" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1503,19 +1537,21 @@
       </c>
       <c r="AB1" s="25"/>
       <c r="AC1" s="25"/>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
       <c r="AG1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1612,9 +1648,17 @@
       <c r="AF2" t="s">
         <v>55</v>
       </c>
-      <c r="AG2" s="6"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG2" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="AH2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -1675,8 +1719,15 @@
       <c r="AF3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -1737,8 +1788,13 @@
       <c r="AF4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+      <c r="AI4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -1795,8 +1851,13 @@
       <c r="AF5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG5" s="22"/>
+      <c r="AH5" s="22"/>
+      <c r="AI5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
@@ -1863,8 +1924,13 @@
       <c r="AF6" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>58</v>
       </c>
@@ -1927,8 +1993,17 @@
       <c r="AF7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG7" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="AH7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>62</v>
       </c>
@@ -1991,8 +2066,15 @@
       <c r="AF8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG8" s="22"/>
+      <c r="AH8" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>67</v>
       </c>
@@ -2061,8 +2143,17 @@
       <c r="AF9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG9" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="AH9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>70</v>
       </c>
@@ -2126,8 +2217,13 @@
       <c r="AF10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG10" s="22"/>
+      <c r="AH10" s="22"/>
+      <c r="AI10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>73</v>
       </c>
@@ -2186,8 +2282,13 @@
       <c r="AF11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG11" s="22"/>
+      <c r="AH11" s="22"/>
+      <c r="AI11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="26"/>
@@ -2256,8 +2357,15 @@
       <c r="AF12" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG12" s="22"/>
+      <c r="AH12" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="26"/>
@@ -2330,8 +2438,13 @@
       <c r="AF13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG13" s="22"/>
+      <c r="AH13" s="22"/>
+      <c r="AI13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="26"/>
@@ -2396,8 +2509,13 @@
       <c r="AF14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG14" s="22"/>
+      <c r="AH14" s="22"/>
+      <c r="AI14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="26"/>
@@ -2456,8 +2574,17 @@
       <c r="AF15" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG15" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH15" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="26"/>
@@ -2514,8 +2641,13 @@
       <c r="AF16" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG16" s="22"/>
+      <c r="AH16" s="22"/>
+      <c r="AI16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="26"/>
@@ -2578,8 +2710,15 @@
       <c r="AF17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG17" s="22"/>
+      <c r="AH17" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C18" s="26" t="s">
         <v>91</v>
       </c>
@@ -2652,8 +2791,13 @@
       <c r="AF18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG18" s="22"/>
+      <c r="AH18" s="22"/>
+      <c r="AI18" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="2" t="s">
@@ -2722,8 +2866,13 @@
       <c r="AF19" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG19" s="22"/>
+      <c r="AH19" s="22"/>
+      <c r="AI19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="2" t="s">
@@ -2782,8 +2931,17 @@
       <c r="AF20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG20" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
       <c r="E21" s="2" t="s">
@@ -2846,8 +3004,15 @@
       <c r="AF21" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG21" s="22"/>
+      <c r="AH21" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C22" s="26"/>
       <c r="D22" s="26" t="s">
         <v>36</v>
@@ -2906,8 +3071,13 @@
       <c r="AF22" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG22" s="22"/>
+      <c r="AH22" s="22"/>
+      <c r="AI22" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
       <c r="E23" s="2" t="s">
@@ -2972,8 +3142,13 @@
       <c r="AF23" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG23" s="22"/>
+      <c r="AH23" s="22"/>
+      <c r="AI23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
       <c r="E24" s="2" t="s">
@@ -3034,8 +3209,17 @@
       <c r="AF24" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG24" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH24" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C25" s="26" t="s">
         <v>104</v>
       </c>
@@ -3100,8 +3284,13 @@
       <c r="AF25" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG25" s="22"/>
+      <c r="AH25" s="22"/>
+      <c r="AI25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
       <c r="E26" t="s">
@@ -3164,8 +3353,13 @@
       <c r="AF26" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG26" s="22"/>
+      <c r="AH26" s="22"/>
+      <c r="AI26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C27" s="26"/>
       <c r="D27" s="26" t="s">
         <v>36</v>
@@ -3224,8 +3418,15 @@
       <c r="AF27" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG27" s="22"/>
+      <c r="AH27" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
       <c r="E28" t="s">
@@ -3290,8 +3491,13 @@
       <c r="AF28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG28" s="22"/>
+      <c r="AH28" s="22"/>
+      <c r="AI28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C29" s="26" t="s">
         <v>115</v>
       </c>
@@ -3354,8 +3560,13 @@
       <c r="AF29" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG29" s="22"/>
+      <c r="AH29" s="22"/>
+      <c r="AI29" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
       <c r="E30" t="s">
@@ -3420,8 +3631,13 @@
       <c r="AF30" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG30" s="22"/>
+      <c r="AH30" s="22"/>
+      <c r="AI30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
       <c r="E31" t="s">
@@ -3490,8 +3706,17 @@
       <c r="AF31" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG31" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="AH31" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
       <c r="E32" t="s">
@@ -3544,8 +3769,13 @@
       <c r="AF32" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="33" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AG32" s="22"/>
+      <c r="AH32" s="22"/>
+      <c r="AI32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
       <c r="E33" t="s">
@@ -3612,8 +3842,15 @@
       <c r="AF33" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AG33" s="22"/>
+      <c r="AH33" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C34" s="26"/>
       <c r="D34" s="26" t="s">
         <v>36</v>
@@ -3678,8 +3915,13 @@
       <c r="AF34" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AG34" s="22"/>
+      <c r="AH34" s="22"/>
+      <c r="AI34" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="35" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
       <c r="E35" t="s">
@@ -3734,8 +3976,13 @@
       <c r="AF35" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="36" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AG35" s="22"/>
+      <c r="AH35" s="22"/>
+      <c r="AI35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
       <c r="E36" t="s">
@@ -3792,8 +4039,17 @@
       <c r="AF36" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="37" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AG36" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="AH36" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C37" s="26" t="s">
         <v>129</v>
       </c>
@@ -3852,8 +4108,15 @@
       <c r="AF37" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AG37" s="22"/>
+      <c r="AH37" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
       <c r="E38" t="s">
@@ -3908,8 +4171,17 @@
       <c r="AF38" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="39" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AG38" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="AH38" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
       <c r="E39" t="s">
@@ -3984,8 +4256,13 @@
       <c r="AF39" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="40" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AG39" s="22"/>
+      <c r="AH39" s="22"/>
+      <c r="AI39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C40" s="26"/>
       <c r="D40" s="26" t="s">
         <v>36</v>
@@ -4048,8 +4325,13 @@
       <c r="AF40" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="41" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AG40" s="22"/>
+      <c r="AH40" s="22"/>
+      <c r="AI40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C41" s="26"/>
       <c r="D41" s="26"/>
       <c r="E41" t="s">
@@ -4104,8 +4386,15 @@
       <c r="AF41" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="42" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AG41" s="22"/>
+      <c r="AH41" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
       <c r="E42" t="s">
@@ -4162,8 +4451,13 @@
       <c r="AF42" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="43" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AG42" s="22"/>
+      <c r="AH42" s="22"/>
+      <c r="AI42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C43" s="26" t="s">
         <v>136</v>
       </c>
@@ -4231,7 +4525,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" t="s">
@@ -4291,7 +4585,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C45" s="26"/>
       <c r="D45" s="26" t="s">
         <v>36</v>
@@ -4353,7 +4647,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C46" s="26"/>
       <c r="D46" s="26"/>
       <c r="E46" t="s">
@@ -4423,7 +4717,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C47" s="26" t="s">
         <v>144</v>
       </c>
@@ -4487,7 +4781,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C48" s="26"/>
       <c r="D48" s="26"/>
       <c r="E48" t="s">
@@ -8658,7 +8952,29 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="460">
+  <mergeCells count="482">
+    <mergeCell ref="AH38:AH40"/>
+    <mergeCell ref="AH41:AH42"/>
+    <mergeCell ref="AG38:AG42"/>
+    <mergeCell ref="AH21:AH23"/>
+    <mergeCell ref="AG20:AG23"/>
+    <mergeCell ref="AH24:AH26"/>
+    <mergeCell ref="AH27:AH30"/>
+    <mergeCell ref="AG24:AG30"/>
+    <mergeCell ref="AH31:AH32"/>
+    <mergeCell ref="AH33:AH35"/>
+    <mergeCell ref="AG31:AG35"/>
+    <mergeCell ref="AG36:AG37"/>
+    <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="AH3:AH6"/>
+    <mergeCell ref="AG2:AG6"/>
+    <mergeCell ref="AG7:AG8"/>
+    <mergeCell ref="AH9:AH11"/>
+    <mergeCell ref="AH12:AH14"/>
+    <mergeCell ref="AG9:AG14"/>
+    <mergeCell ref="AH15:AH16"/>
+    <mergeCell ref="AH17:AH19"/>
+    <mergeCell ref="AG15:AG19"/>
     <mergeCell ref="AE34:AE36"/>
     <mergeCell ref="AD34:AD37"/>
     <mergeCell ref="AE38:AE40"/>

</xml_diff>